<commit_message>
chgt xxx colonne export + selection ihm
</commit_message>
<xml_diff>
--- a/src/main/resources/template-segur-requirement-export-avec-colonnes-prepub-modifie.xlsx
+++ b/src/main/resources/template-segur-requirement-export-avec-colonnes-prepub-modifie.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\flabatie\Documents\ENV-ANS\19-PLUGIN-SQUASH\squash-plugin\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cjuillard\Documents\segur\squash-convergence-plugin\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EC2D3EF-0E0F-4D16-B3CB-214D352B221E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7367688-22C9-482D-BB7B-08EBED09D226}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Exigences" sheetId="1" r:id="rId1"/>
@@ -184,9 +184,6 @@
     <t>MSS/CDA.01.01.01</t>
   </si>
   <si>
-    <t>Chapitre</t>
-  </si>
-  <si>
     <t>ID</t>
   </si>
   <si>
@@ -197,6 +194,9 @@
   </si>
   <si>
     <t>Commentaire</t>
+  </si>
+  <si>
+    <t>Chapitrezzzzzzzzzzz</t>
   </si>
 </sst>
 </file>
@@ -715,60 +715,60 @@
   <sheetPr codeName="Feuil5"/>
   <dimension ref="A1:AK2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Z1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="AC2" sqref="AC2"/>
+      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.28515625" defaultRowHeight="15.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.25" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="13.2109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="37.92578125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="35.2109375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="66.42578125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="15.0703125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="12.2109375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="18.5703125" style="5" customWidth="1"/>
-    <col min="8" max="8" width="66.42578125" style="6" customWidth="1"/>
-    <col min="9" max="9" width="18.5703125" style="7" customWidth="1"/>
-    <col min="10" max="10" width="30.5703125" style="6" customWidth="1"/>
-    <col min="11" max="11" width="18.5703125" style="7" customWidth="1"/>
-    <col min="12" max="12" width="30.5703125" style="6" customWidth="1"/>
-    <col min="13" max="13" width="18.5703125" style="7" customWidth="1"/>
-    <col min="14" max="14" width="30.5703125" style="6" customWidth="1"/>
-    <col min="15" max="15" width="18.5703125" style="7" customWidth="1"/>
-    <col min="16" max="16" width="30.5703125" style="6" customWidth="1"/>
-    <col min="17" max="17" width="18.5703125" style="7" customWidth="1"/>
-    <col min="18" max="18" width="30.5703125" style="6" customWidth="1"/>
-    <col min="19" max="19" width="18.5703125" style="7" customWidth="1"/>
-    <col min="20" max="20" width="30.5703125" style="6" customWidth="1"/>
-    <col min="21" max="21" width="18.5703125" style="7" customWidth="1"/>
-    <col min="22" max="22" width="30.5703125" style="6" customWidth="1"/>
-    <col min="23" max="23" width="18.5703125" style="7" customWidth="1"/>
-    <col min="24" max="24" width="30.5703125" style="6" customWidth="1"/>
-    <col min="25" max="25" width="18.5703125" style="7" customWidth="1"/>
-    <col min="26" max="26" width="30.5703125" style="6" customWidth="1"/>
-    <col min="27" max="27" width="18.5703125" style="7" customWidth="1"/>
-    <col min="28" max="30" width="30.5703125" style="6" customWidth="1"/>
-    <col min="31" max="34" width="15.2109375" style="21" customWidth="1"/>
-    <col min="35" max="35" width="40.28515625" style="21" customWidth="1"/>
-    <col min="36" max="36" width="52.28515625" style="21" customWidth="1"/>
-    <col min="37" max="37" width="13.92578125" style="21" customWidth="1"/>
-    <col min="38" max="16384" width="9.28515625" style="8"/>
+    <col min="1" max="1" width="13.25" style="2" customWidth="1"/>
+    <col min="2" max="2" width="37.9140625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="35.25" style="2" customWidth="1"/>
+    <col min="4" max="4" width="66.4140625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="15.08203125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="12.25" style="2" customWidth="1"/>
+    <col min="7" max="7" width="18.58203125" style="5" customWidth="1"/>
+    <col min="8" max="8" width="66.4140625" style="6" customWidth="1"/>
+    <col min="9" max="9" width="18.58203125" style="7" customWidth="1"/>
+    <col min="10" max="10" width="30.58203125" style="6" customWidth="1"/>
+    <col min="11" max="11" width="18.58203125" style="7" customWidth="1"/>
+    <col min="12" max="12" width="30.58203125" style="6" customWidth="1"/>
+    <col min="13" max="13" width="18.58203125" style="7" customWidth="1"/>
+    <col min="14" max="14" width="30.58203125" style="6" customWidth="1"/>
+    <col min="15" max="15" width="18.58203125" style="7" customWidth="1"/>
+    <col min="16" max="16" width="30.58203125" style="6" customWidth="1"/>
+    <col min="17" max="17" width="18.58203125" style="7" customWidth="1"/>
+    <col min="18" max="18" width="30.58203125" style="6" customWidth="1"/>
+    <col min="19" max="19" width="18.58203125" style="7" customWidth="1"/>
+    <col min="20" max="20" width="30.58203125" style="6" customWidth="1"/>
+    <col min="21" max="21" width="18.58203125" style="7" customWidth="1"/>
+    <col min="22" max="22" width="30.58203125" style="6" customWidth="1"/>
+    <col min="23" max="23" width="18.58203125" style="7" customWidth="1"/>
+    <col min="24" max="24" width="30.58203125" style="6" customWidth="1"/>
+    <col min="25" max="25" width="18.58203125" style="7" customWidth="1"/>
+    <col min="26" max="26" width="30.58203125" style="6" customWidth="1"/>
+    <col min="27" max="27" width="18.58203125" style="7" customWidth="1"/>
+    <col min="28" max="30" width="30.58203125" style="6" customWidth="1"/>
+    <col min="31" max="34" width="15.25" style="21" customWidth="1"/>
+    <col min="35" max="35" width="40.25" style="21" customWidth="1"/>
+    <col min="36" max="36" width="52.25" style="21" customWidth="1"/>
+    <col min="37" max="37" width="13.9140625" style="21" customWidth="1"/>
+    <col min="38" max="16384" width="9.25" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:37" s="1" customFormat="1" ht="56.25" customHeight="1">
       <c r="A1" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="C1" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E1" s="9" t="s">
         <v>2</v>
@@ -843,10 +843,10 @@
         <v>24</v>
       </c>
       <c r="AC1" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AD1" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AE1" s="23" t="s">
         <v>25</v>

</xml_diff>